<commit_message>
[ADDITIONAL SCRAPING] added scraping code for extra browling attributes and excel sheets
</commit_message>
<xml_diff>
--- a/bin/sheets/main_db/teams/AFG/PlayerPerformance_3665.xlsx
+++ b/bin/sheets/main_db/teams/AFG/PlayerPerformance_3665.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ODI Batting" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ODI Bowling" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ODI Batting Extra" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ODI Bowling Extra" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -12508,10 +12509,6 @@
           <t>4326</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>NO</t>
@@ -12524,457 +12521,758 @@
           <t>4332</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>4335</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4340</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>7.05%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4348</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.69%</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>4377</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.52%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>4378</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>16.00%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>4379</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>20.08%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>4444</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1.05%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>4446</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>4448</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12.03%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>4537</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>9.30%</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>4538</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>4539</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>6</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>4582</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3.62%</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>4585</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4588</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>24.82%</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>4671</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>4674</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>7</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>17.98%</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>4675</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MATCH_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>MAIDEN_OVERS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PERCENT_WICKETS_OF_ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>4323</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>4326</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4335</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
+          <t>4332</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4340</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>6</v>
+          <t>4335</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>7.05%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4348</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
+          <t>4340</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0.69%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4377</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>7</v>
+          <t>4348</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0.52%</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4378</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+          <t>4377</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>16.00%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4379</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>7</v>
+          <t>4378</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>20.08%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4444</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>5</v>
+          <t>4379</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1.05%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4446</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>4444</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4448</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>6</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>12.03%</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
+          <t>4446</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4537</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>6</v>
+          <t>4448</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>9.30%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>10.00%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4538</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>4537</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4539</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>6</v>
-      </c>
+          <t>4538</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4582</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>5</v>
+          <t>4539</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>3.62%</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4585</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>6</v>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>4582</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>40.00%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4588</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>6</v>
+          <t>4585</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>24.82%</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4671</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>NO</t>
+          <t>4588</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4674</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>7</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>17.98%</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
+          <t>4671</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -12984,13 +13282,6 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>